<commit_message>
Creating and returning a Recipy obj from query
</commit_message>
<xml_diff>
--- a/backend/dbOverview.xlsx
+++ b/backend/dbOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Code\repos\thriftyHelper\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3807AB65-CBF3-4A01-B358-E4851AF3B73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B195CD1-29DF-4CE3-9BE5-5DAE9EA1B110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{E73CE52E-63C9-430C-8ECC-EEE6B0E15140}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8268" windowHeight="12360" xr2:uid="{E73CE52E-63C9-430C-8ECC-EEE6B0E15140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
-    <t>Igredients</t>
-  </si>
-  <si>
     <t>ing_id</t>
   </si>
   <si>
@@ -59,18 +56,12 @@
     <t>p/unit</t>
   </si>
   <si>
-    <t>recipies</t>
-  </si>
-  <si>
     <t>rec_id</t>
   </si>
   <si>
     <t>desc</t>
   </si>
   <si>
-    <t>ingredientsToRes</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -87,6 +78,15 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>ingredientsInRes</t>
+  </si>
+  <si>
+    <t>stored_recipies</t>
+  </si>
+  <si>
+    <t>stored_ingredients</t>
   </si>
 </sst>
 </file>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B405BAE-359B-4603-89C8-E5FFD8E5D815}">
-  <dimension ref="B3:I10"/>
+  <dimension ref="B3:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,102 +449,120 @@
     <col min="6" max="6" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>